<commit_message>
some more info from deej
</commit_message>
<xml_diff>
--- a/data/bios.xlsx
+++ b/data/bios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12040" yWindow="0" windowWidth="16740" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="202">
   <si>
     <t>Future Rock</t>
   </si>
@@ -138,21 +138,6 @@
     <t>http://russliquid.com/wp-content/uploads/2013/05/Russ-Liquid-Promo-Photo.jpg</t>
   </si>
   <si>
-    <t>http://cherublamusica.com/</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/Cherublamusica</t>
-  </si>
-  <si>
-    <t>https://soundcloud.com/cherublamusica</t>
-  </si>
-  <si>
-    <t>http://cherub.bandcamp.com/</t>
-  </si>
-  <si>
-    <t>http://cherublamusica.com/wp-content/uploads/2012/09/cherub131.jpg</t>
-  </si>
-  <si>
     <t>http://www.blueboyproductions.net</t>
   </si>
   <si>
@@ -279,9 +264,6 @@
     <t>http://musicisadirtyword.com/index/wp-content/uploads/2011/11/cropped-1027112049b.jpg</t>
   </si>
   <si>
-    <t>Cosmal's Community Stage</t>
-  </si>
-  <si>
     <t>http://thecosmalshow.com/</t>
   </si>
   <si>
@@ -312,9 +294,6 @@
     <t>https://www.youtube.com/watch?v=XTbwzz9Cqo4</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=XlZtvEM5mf4</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=a0TCJhjlNSA</t>
   </si>
   <si>
@@ -358,12 +337,6 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=pS1SqQB62tg</t>
-  </si>
-  <si>
-    <t>Love and Light (not announced)</t>
-  </si>
-  <si>
-    <t>CHERUB (not announced)</t>
   </si>
   <si>
     <t>Colony Vegetable</t>
@@ -429,11 +402,6 @@
     <t>A morphing 4-piece from Southern NH, these boys like to mix things up, taking influences across the entire music spectrum and blending them into a coherent, melodic and often outrageous sound. Add a gratuitous amount of black lights, a dazzling light show and you have that which is the BlackLight Ruckus</t>
   </si>
   <si>
-    <t>Cherub is a sexy, avante garde, electro-pop duo that is the dance love-child of 80's funk, and pop-music from the future. The members of Cherub, Jordan Kelley and Jason Huber, share a love for honest original music and vibrant live performance, with a common goal to share a little bit of sex, a little bit of drugs, and a whole lot of love with people across the globe. Cherub's music is a fresh electrified take on risqué pop music that brings to mind timeless artists like Prince, Zapp and Roger, and more contemporary artists like Pharrel, and The Dream. With a live show that is bouncing with energy, Cherub dances their way into the hearts of audiences from the first falsetto hook, until the very last delay filters out.
-After receiving a warm response worldwide to the digital release on the band's first record, Man of the Hour, and touring throughout the US and Mexico, Cherub has returned to the studio to complete work on their second album, which is scheduled for release in early 2012. This new batch of Cherub songs brings a fresh, uptempo electro feel to the familiar pop sensibilities showcased on their first record. Jordan Kelley's clever songwriting and silky smooth falsetto are complimented perfectly by Jason Huber's production and tube-driven guitar work. Cherub's debut album Man of the Hour is available for free download at ElmandOak.com, and stay tuned for more news regarding Cherub's new album coming out early next year.
-Cherub's versatility in songwriting and dance music production blurs conventional genre barriers. Ranging from grooving heartfelt ballads to risqué club bangers, Cherub takes the throwback vibes of old drum machines and washed out keyboards, and marries them with timeless songwriting and a very modern approach to music production and performance. Playful guitar licks and lush synthesizer textures dance around in the mix, as listeners are treated to sing-a-long hook after hook the entire way through the tunes.</t>
-  </si>
-  <si>
     <t>Russ Liquid is the future-vintage groove-blasting maestro who has stirred the souls and minds of the electronic music world. Renowned for his ingenious compositional approach, this cosmic virtuoso and imprints a prophetic musical experience on his audiences. He detonates explosive beatscapes, seamlessly adding flourishes of instrumental color and emotion; all while drawing from an endlessly diverse sonic palette.
 In only a short time, Mr. Liquid has developed a reputation for radiating a sonic supernova of genre-bending beats on the dancefloor, captivating audiences with passionate live instrumental performances across the U.S. and beyond. In 2012, the member of the Headtron crew's dynamic, multi-instrumental, experience was unleashed on some of the most innovative events and festivals around the globe including: Coachella, Symbiosis Gathering, Lightning In A Bottle, Shambhala, Sonic Bloom, Envision Festival (Costa Rica), and Eclipse Festival (Australia).
 In February of 2013, Russ resumes his destiny to break musical boundaries and transcend expectations with Foreign Frequency, his debut full length album on STS9's 1320 Records. Foreign Frequency transports listeners on an inter- dimensional adventure to the deepest circles of his musical universe, steering audiences into an expansive world of visceral beats, laced with spiraling instrumental accompaniments, and adorned with melodies that only a masterful improvisationalist could manifest.
@@ -471,13 +439,219 @@
   </si>
   <si>
     <t>Cosmal is a one man LIVE music performance involving the layering and looping of different instruments, progressive build ups, and rampant improvisation. Layering sounds to create the energy of a full band or DJ, improvising and swaying between genres, Cosmal takes you on a mystical journey through space and time, and oh yea, music! Performances always feature Live Painter Ali Laz. Conscious Minded Media for Conscious Minded People ranging from World and Trance to Fusion and Rock. This is a completely live act people, not a DJ set! Good Vibes required, Shirts and Shoes optional! Since late 2010, Cosmal has performed at over 35 music festivals including Rock N Roll Resort, Heads in Harmony, Freedom of Expression, Bonnaroo, Forest Fest and more, having shared bills with Shpongle, Ott, Papadosio, Zach Deputy, Dopapod, Lettuce, and many more. Cosmal has opened for acts like Big Gigantic and Conspirator, as well as having performed with visionary artist Alex Grey. Cosmal was featured in Relix Magazine and Sampler CD January/February 2012!</t>
+  </si>
+  <si>
+    <t>Marco Benevento</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Brooklyn, NY</t>
+  </si>
+  <si>
+    <t>Chicago, IL</t>
+  </si>
+  <si>
+    <t>Jimkata</t>
+  </si>
+  <si>
+    <t>Ithaca, NY</t>
+  </si>
+  <si>
+    <t>http://jimkata.com</t>
+  </si>
+  <si>
+    <t>http://marcobenevento.com</t>
+  </si>
+  <si>
+    <t>Denver, CO</t>
+  </si>
+  <si>
+    <t>Love and Light</t>
+  </si>
+  <si>
+    <t>Reno, NV</t>
+  </si>
+  <si>
+    <t>Oakland, CA</t>
+  </si>
+  <si>
+    <t>The Manhattan Project</t>
+  </si>
+  <si>
+    <t>Rochester, NY</t>
+  </si>
+  <si>
+    <t>http://themanhattanprojectlive.com</t>
+  </si>
+  <si>
+    <t>Boston, MA</t>
+  </si>
+  <si>
+    <t>Keene, NH</t>
+  </si>
+  <si>
+    <t>Lakes Region, NH</t>
+  </si>
+  <si>
+    <t>Scranton, PA</t>
+  </si>
+  <si>
+    <t>Of The Trees</t>
+  </si>
+  <si>
+    <t>Portland, ME</t>
+  </si>
+  <si>
+    <t>MUN</t>
+  </si>
+  <si>
+    <t>http://munmusic.bandcamp.com</t>
+  </si>
+  <si>
+    <t>Rogue Chimp</t>
+  </si>
+  <si>
+    <t>http://roguechimpmusic.com</t>
+  </si>
+  <si>
+    <t>Cosmal</t>
+  </si>
+  <si>
+    <t>Massapequa, NY</t>
+  </si>
+  <si>
+    <t>KONG</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/KongTheBand</t>
+  </si>
+  <si>
+    <t>Voyagers!</t>
+  </si>
+  <si>
+    <t>Nashua, NH</t>
+  </si>
+  <si>
+    <t>https://soundcloud.com/voyagersmusicmix</t>
+  </si>
+  <si>
+    <t>Nasstronaut</t>
+  </si>
+  <si>
+    <t>http://marcobenevento.com/wp-content/uploads/2012/06/120605_benvento_179-Edit.jpg</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/marco.benevento</t>
+  </si>
+  <si>
+    <t>https://soundcloud.com/ofthetrees</t>
+  </si>
+  <si>
+    <t>For more than a decade pianist/sound-sculptor/songwriter Marco Benevento has been amassing an extensive resume of composition and collaboration. His studio albums have set forth a vision for music that connects the dots between Explosions In The Sky and Tortoise on one side, Brian Eno and Brad Mehldau on the other, while in the live setting his performances reverberate with pulsating dance rock energy. The 34-year old artist takes the next step forward in this evolution with his latest album, TigerFace, on which he paints his songs in a myriad of sonic colors, shimmering with acoustic piano, synths and analog keyboards. The tunes themselves seemingly conceptualized from every wisp of melody, hook and cadence that's ever tickled his ear.
+Recorded and mixed by Tom Biller (Silversun Pickups, Fiona Apple) and Bryce Goggin (Pavement, Akron/Family), TigerFace features a stellar cast of musicians recruited to help capture his ideas, including drummers Matt Chamberlain (Bill Frisell, Pearl Jam), John McEntire (Tortoise, The Sea &amp; The Cake) and Andrew Barr (The Barr Brothers), bassists Dave Dreiwitz (Ween), Reed Mathis (Tea Leaf Green) and Mike Gordon (Phish), violinist Ali Helnwein (Traction Avenue Chamber Orchestra) and saxophonist Stuart Bogie (Antibalas, Superhuman Happiness). For the first time, Benevento presents vocals, inviting Kalmia Traver (Rubblebucket) to sing on the infectious dance rock rave-up Limbs Of A Pine and the pastoral psych rock meditation This Is How It Goes. Other standouts include the angelic Arcade Fire meets The Flaming Lips anthem "Eagle Rock," the soaring garage psychedelia of Going West, the piano riff rock jaunt Escape Horse, and the happily lilting Fireworks.
+As anybody who's seen Benevento perform live can attest, the pianist is a satellite to the muse with eyes closed, smile wide across his face and fingers free-flowing across the keys. Indeed, TigerFace, is the commitment to this pursuit; a record that rides the yes wave and in the process becomes a soundtrack for fellow travelers with their eyes set on the horizon.</t>
+  </si>
+  <si>
+    <t>http://www.jimkata.com/gallery/full/2.jpg</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/jimkatamusic</t>
+  </si>
+  <si>
+    <t>https://soundcloud.com/jimkata</t>
+  </si>
+  <si>
+    <t>http://jimkata.bandcamp.com/</t>
+  </si>
+  <si>
+    <t>Since exploding on to the scene in 2010, The Manhattan Project has become one of the fastest growing live electronic duos in the northeast. Selling out shows regionally, and with bands like Lotus, Conspirator and BioDiesel, they've gained national attention as a band on the rise. Drawing influences from house, dub, drum n bass, techno and lounge, The Manhattan Project brings sophistication to the dance floor with their original compositions, high energy beats and mind melting textures. Armed with an arsenal of keyboards, synths, electronic and acoustic percussion, they seamlessly merge analogue and digital sounds to create a sonic boomtronic style all their own. Live visuals by NGB and epic light shows bring the concert experience to a new level, and have earned them the reputation of a must-see live band.
+In just a short time, the duo has toured all over the northeast, playing consistently to large crowds at dance clubs, live music venues and late night festival slots, collaborated with top regional DJ's and MC's, performed live sets on top alternative radio stations and have gained loyal fans through word of mouth and high energy live shows.
+Their new EP 'Atomic Bomb Party Vol. 2' was just released in April for free download to great reviews and is embraced by DJ and live music fans alike! The Manhattan Project features Shawn Drogan on drums and electronics, and Charlie Lindner on keyboards and synths.
+The Manhattan Project has opened for Lotus, Conspirator, Future Rock, BioDiesel, Ozric Tentacles, Ludachrist, Communist Party and more</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/themanhattanprojectlive</t>
+  </si>
+  <si>
+    <t>https://soundcloud.com/themanhattanprojectlive</t>
+  </si>
+  <si>
+    <t>http://themanhattanprojectlive.bandcamp.com/</t>
+  </si>
+  <si>
+    <t>https://sphotos-b.xx.fbcdn.net/hphotos-ash3/s720x720/535471_10152538765760109_2119962962_n.jpg</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/ofthetrees</t>
+  </si>
+  <si>
+    <t>https://sphotos-b.xx.fbcdn.net/hphotos-ash3/541400_383088368390025_2044082377_n.jpg</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/MUN.NYC</t>
+  </si>
+  <si>
+    <t>MUN is a quartet of versatile musicians based out of Brooklyn, NYC. Starting out as an all-improv outfit playing the New York underground warehouse circuit and summer festivals across the northeast, MUN has evolved their dancey electronic sound into a psychedelic pallet of jazz, rock, funk, and drum n bass. With their willingness to consistently develop their craft, MUN brings a quality experience to listeners at every show.</t>
+  </si>
+  <si>
+    <t>https://fbcdn-sphotos-b-a.akamaihd.net/hphotos-ak-ash3/164199_626684860691684_674483533_n.jpg</t>
+  </si>
+  <si>
+    <t>https://soundcloud.com/munmusic</t>
+  </si>
+  <si>
+    <t>https://soundcloud.com/roguechimp</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/roguechimp</t>
+  </si>
+  <si>
+    <t>http://roguechimp.bandcamp.com/</t>
+  </si>
+  <si>
+    <t>Rogue Chimp's music is a unique combination of jazz/fusion, prog/funk, classical/techno, and world music, with electronic inspired grooves using violin and synths interwoven throughout.</t>
+  </si>
+  <si>
+    <t>https://c-ugc-ak.secure.static-rootmusic.com/bandpage-photos/0/7326/143483415063183360/large.jpg</t>
+  </si>
+  <si>
+    <t>Kong brings the thunderfunk, genetically engineered to plaster the walls of your ears with visual groove product placement. These five musicians from diverse backgrounds come together to bring back the feeling of your first head nod.</t>
+  </si>
+  <si>
+    <t>https://sphotos-a.xx.fbcdn.net/hphotos-prn1/265106_166153456785986_5460315_n.jpg</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/Voyagersmusic</t>
+  </si>
+  <si>
+    <t>What started as a weekly jam session between best friends, a shared dropbox account, and a craigslist ad, quickly became an adventure into self expression and brotherhood.</t>
+  </si>
+  <si>
+    <t>https://fbcdn-sphotos-c-a.akamaihd.net/hphotos-ak-prn1/602123_611637212186901_1885702719_n.jpg</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/NasstronautMusic</t>
+  </si>
+  <si>
+    <t>Disco-House. NuDisco. Tech-House. Wonky-Disco. Deep-House.</t>
+  </si>
+  <si>
+    <t>https://fbcdn-sphotos-e-a.akamaihd.net/hphotos-ak-ash4/486438_484602951602742_946192828_n.jpg</t>
+  </si>
+  <si>
+    <t>Of the Trees is Tyler Coombs; electronic music producer hailing from Portland, Maine. Melding strong influences from hip hop, downtempo, and EDM - Of the Trees has crafted his own special blend of bass-heavy beats that keep the listening (and live) experience full of surprising twists and turns. At just 21 years old and currently in his first year of performing live - Of the Trees has made a significant impact on the East Coast bass music scene and isn't slowing down any time soon. He has shared stages with the likes of Kill the Noise, Opiuo, RJD2, Paper Diamond, Phutureprimitive, Minnesota, and many more widely renowned artists. His debut EP Threshold was released on 12/12/12 via Gravitas Recordings and immediately gained attention from some of the best electronic music blogs in the country; including Glitchhop.net, The Untz, LostinSound, and The Brain Trust.</t>
+  </si>
+  <si>
+    <t>Now touring to support their innovative, fan-funded record Die Digital, Jimkata has been a mainstay of the Northeast for years. Recent traction stemming from the rise of electronic dance music (EDM) has afforded them the opportunity to continue expanding their signature brand of song-oriented electro-rock. Analog synthesizers and heavy bass notes fill the electronic role, while big guitars create space for shredding within the structure of pure indie rock. Over the years they have consistently backed up their reputation for creating high-energy dance parties at such music festivals as Summer Camp, Camp Bisco, and Mountain Jam alongside such diverse acts as Primus, LCD Soundsystem, Pretty Lights &amp; The Roots. For Jimkata fans, however, the show doesn't end when the lights come up. Jimkata's relevant, quotable lyrics create music not just for the fleeting moments, but for the lifestyle of an entire generation.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -513,10 +687,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Lucida Grande"/>
+    </font>
+    <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Trebuchet MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -550,7 +731,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -565,13 +746,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -916,587 +1106,773 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="F17" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="G5" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="58.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" customWidth="1"/>
-    <col min="5" max="5" width="39" customWidth="1"/>
-    <col min="6" max="6" width="65.1640625" customWidth="1"/>
-    <col min="7" max="7" width="36.83203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="108.1640625" customWidth="1"/>
+    <col min="1" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="4" max="4" width="58.6640625" customWidth="1"/>
+    <col min="5" max="5" width="42.5" customWidth="1"/>
+    <col min="6" max="6" width="41.83203125" customWidth="1"/>
+    <col min="7" max="7" width="65.1640625" customWidth="1"/>
+    <col min="8" max="8" width="44.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="108.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="409.6">
+      <c r="A2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="270">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="273">
+      <c r="A4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="409">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="345">
+      <c r="A6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="409">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="409">
+      <c r="A8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="300">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="90">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="330">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="H10" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="409">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="409">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="409">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="409">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="360">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="120">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="2" t="s">
+    </row>
+    <row r="13" spans="1:9" ht="281">
+      <c r="A13" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="105">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="165">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="409">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="H15" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
+      <c r="I15" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="141">
+      <c r="A16" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="57">
+      <c r="A17" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="330">
+      <c r="A18" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="409">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="120">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="H18" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="409">
+      <c r="A19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="F19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="409">
-      <c r="A10" s="2" t="s">
+      <c r="I19" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="409">
+      <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="195">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="409">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12" s="2" t="s">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60">
-      <c r="A13" s="2" t="s">
+    <row r="21" spans="1:9" ht="85">
+      <c r="A21" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="I21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45">
+      <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="255">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="75">
-      <c r="A15" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="285">
-      <c r="A16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" ht="105">
-      <c r="A18" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" ht="405">
-      <c r="A20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="210">
+      <c r="A23" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="60">
+      <c r="A24" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="240">
+      <c r="A25" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="F25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" ht="405">
+      <c r="G25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="57">
       <c r="A26" s="2" t="s">
-        <v>113</v>
+        <v>164</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="409">
+        <v>194</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="90">
       <c r="A27" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="G32" s="6"/>
+        <v>117</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" ht="29">
+      <c r="A29" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D29" t="s">
+        <v>197</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="I29" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I30" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G12" r:id="rId1" display="The Durian, the spiny, stinky fruit, is both famous and infamous in its native home of South-East Asia.  Eliciting emotions that range from respect to disgust to adoration, the fruit has earned the nickname, &quot;King of Fruits,&quot; and has been banned in many h"/>
+    <hyperlink ref="H19" r:id="rId1" display="The Durian, the spiny, stinky fruit, is both famous and infamous in its native home of South-East Asia.  Eliciting emotions that range from respect to disgust to adoration, the fruit has earned the nickname, &quot;King of Fruits,&quot; and has been banned in many h"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C8" r:id="rId3"/>
+    <hyperlink ref="E13" r:id="rId4"/>
+    <hyperlink ref="F16" r:id="rId5"/>
+    <hyperlink ref="C17" r:id="rId6"/>
+    <hyperlink ref="D21" r:id="rId7"/>
+    <hyperlink ref="E26" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
add cyborg trio to data
</commit_message>
<xml_diff>
--- a/data/bios.xlsx
+++ b/data/bios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="14220" yWindow="200" windowWidth="14360" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="209">
   <si>
     <t>Future Rock</t>
   </si>
@@ -645,13 +645,34 @@
   </si>
   <si>
     <t>Now touring to support their innovative, fan-funded record Die Digital, Jimkata has been a mainstay of the Northeast for years. Recent traction stemming from the rise of electronic dance music (EDM) has afforded them the opportunity to continue expanding their signature brand of song-oriented electro-rock. Analog synthesizers and heavy bass notes fill the electronic role, while big guitars create space for shredding within the structure of pure indie rock. Over the years they have consistently backed up their reputation for creating high-energy dance parties at such music festivals as Summer Camp, Camp Bisco, and Mountain Jam alongside such diverse acts as Primus, LCD Soundsystem, Pretty Lights &amp; The Roots. For Jimkata fans, however, the show doesn't end when the lights come up. Jimkata's relevant, quotable lyrics create music not just for the fleeting moments, but for the lifestyle of an entire generation.</t>
+  </si>
+  <si>
+    <t>The Cyborg Trio</t>
+  </si>
+  <si>
+    <t>http://www.cyborgtrio.com</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/CyborgTrioMusic</t>
+  </si>
+  <si>
+    <t>https://soundcloud.com/thecyborgtrio</t>
+  </si>
+  <si>
+    <t>http://thecyborgtrio.bandcamp.com/</t>
+  </si>
+  <si>
+    <t>The innovative Cyborg Trio are known for their dynamic, psychedelic improvisation and carefully crafted beats. Eric Dudevoir, Sammy B and Tim Nickerson released their fully improvised jam album in early 2009 and since then have been getting more exposure in both the local and national scenes. Their tight, trance-inducing tunes are reminiscent of a DJ; you’ll have to keep reminding yourself that these guys are playing live instruments. For their live shows they bring the crowd through a journey, offering ups and very relieving downs as the beat drops and groove waves travel through the room, filling the venue with good vibes. Listen to the music player below and hear the depth and detail produced from live improvisational jams.</t>
+  </si>
+  <si>
+    <t>https://fbcdn-sphotos-f-a.akamaihd.net/hphotos-ak-ash3/554689_10151025123261453_2122972569_n.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -699,6 +720,11 @@
       <sz val="14"/>
       <name val="Trebuchet MS"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF3D5054"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -731,7 +757,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -762,6 +788,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1106,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="G5" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="I12" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1431,448 +1460,476 @@
     </row>
     <row r="12" spans="1:9" ht="409">
       <c r="A12" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="409">
+      <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="281">
-      <c r="A13" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="281">
+      <c r="A14" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="9" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="105">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:9" ht="105">
+      <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="165">
-      <c r="A15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="165">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="141">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:9" ht="141">
+      <c r="A17" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="57">
-      <c r="A17" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>189</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="57">
+      <c r="A18" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="330">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:9" ht="330">
+      <c r="A19" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="409">
-      <c r="A19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="409">
       <c r="A20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="409">
+      <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H21" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="85">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:9" ht="85">
+      <c r="A22" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H22" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I22" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="45">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:9" ht="45">
+      <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="5" t="s">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="210">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:9" ht="210">
+      <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="60">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:9" ht="60">
+      <c r="A25" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="240">
-      <c r="A25" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="G25" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>70</v>
+        <v>114</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="57">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="240">
       <c r="A26" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>165</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>166</v>
+        <v>71</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="9" t="s">
-        <v>195</v>
+      <c r="G26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="90">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="57">
       <c r="A27" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" s="2"/>
+        <v>164</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>165</v>
+      </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2" t="s">
-        <v>117</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="7" t="s">
-        <v>127</v>
+      <c r="H27" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="90">
       <c r="A28" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="G28" s="2"/>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" ht="29">
-      <c r="A29" s="2" t="s">
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" ht="29">
+      <c r="A30" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>197</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="H30" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I30" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:9">
+      <c r="A31" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="7" t="s">
+      <c r="B31" s="1"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="I30" s="2"/>
+      <c r="I31" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H19" r:id="rId1" display="The Durian, the spiny, stinky fruit, is both famous and infamous in its native home of South-East Asia.  Eliciting emotions that range from respect to disgust to adoration, the fruit has earned the nickname, &quot;King of Fruits,&quot; and has been banned in many h"/>
+    <hyperlink ref="H20" r:id="rId1" display="The Durian, the spiny, stinky fruit, is both famous and infamous in its native home of South-East Asia.  Eliciting emotions that range from respect to disgust to adoration, the fruit has earned the nickname, &quot;King of Fruits,&quot; and has been banned in many h"/>
     <hyperlink ref="C4" r:id="rId2"/>
     <hyperlink ref="C8" r:id="rId3"/>
-    <hyperlink ref="E13" r:id="rId4"/>
-    <hyperlink ref="F16" r:id="rId5"/>
-    <hyperlink ref="C17" r:id="rId6"/>
-    <hyperlink ref="D21" r:id="rId7"/>
-    <hyperlink ref="E26" r:id="rId8"/>
+    <hyperlink ref="E14" r:id="rId4"/>
+    <hyperlink ref="F17" r:id="rId5"/>
+    <hyperlink ref="C18" r:id="rId6"/>
+    <hyperlink ref="D22" r:id="rId7"/>
+    <hyperlink ref="E27" r:id="rId8"/>
+    <hyperlink ref="C12" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>